<commit_message>
Remake resched module, organized Remove unused func in utilities Fix some data holes in data Module resched: done Production
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\SisThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905B7F4F-BDE3-4714-A134-2A26912D7BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA02EBC-D3E5-4134-80FF-3493B19296CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,17 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -201,8 +190,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -349,19 +338,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -373,17 +362,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -393,9 +382,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1316,8 +1304,8 @@
   <dimension ref="A1:M313"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K302" sqref="K302"/>
+      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D280" sqref="D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5953,7 +5941,6 @@
       </c>
       <c r="H192" s="22"/>
       <c r="I192" s="22"/>
-      <c r="J192" s="23"/>
       <c r="K192" s="22"/>
       <c r="L192" s="22"/>
       <c r="M192" s="22"/>
@@ -6445,7 +6432,6 @@
         <v>9648</v>
       </c>
       <c r="H209" s="22"/>
-      <c r="I209" s="23"/>
       <c r="J209" s="22"/>
       <c r="K209" s="22"/>
       <c r="L209" s="22"/>
@@ -6851,7 +6837,6 @@
         <v>7200</v>
       </c>
       <c r="H223" s="22"/>
-      <c r="I223" s="23"/>
       <c r="J223" s="22"/>
       <c r="K223" s="22"/>
       <c r="L223" s="22"/>
@@ -7112,7 +7097,6 @@
         <v>7200</v>
       </c>
       <c r="H232" s="22"/>
-      <c r="I232" s="23"/>
       <c r="J232" s="22"/>
       <c r="K232" s="22"/>
       <c r="L232" s="22"/>
@@ -7170,7 +7154,6 @@
         <v>8640</v>
       </c>
       <c r="H234" s="22"/>
-      <c r="I234" s="23"/>
       <c r="J234" s="22"/>
       <c r="K234" s="22"/>
       <c r="L234" s="22"/>
@@ -7431,7 +7414,6 @@
         <v>6048</v>
       </c>
       <c r="H243" s="22"/>
-      <c r="I243" s="23"/>
       <c r="J243" s="22"/>
       <c r="K243" s="22"/>
       <c r="L243" s="22"/>
@@ -8272,7 +8254,6 @@
         <v>10656</v>
       </c>
       <c r="H272" s="22"/>
-      <c r="I272" s="23"/>
       <c r="J272" s="22"/>
       <c r="K272" s="22"/>
       <c r="L272" s="22"/>
@@ -8462,8 +8443,8 @@
       <c r="C279" s="11">
         <v>900</v>
       </c>
-      <c r="D279" s="3" t="e">
-        <v>#VALUE!</v>
+      <c r="D279" s="3">
+        <v>12000</v>
       </c>
       <c r="E279" s="1">
         <v>39168</v>
@@ -8476,7 +8457,6 @@
       </c>
       <c r="H279" s="22"/>
       <c r="I279" s="22"/>
-      <c r="J279" s="23"/>
       <c r="K279" s="22"/>
       <c r="L279" s="22"/>
       <c r="M279" s="22"/>
@@ -8533,7 +8513,6 @@
         <v>9792</v>
       </c>
       <c r="H281" s="22"/>
-      <c r="I281" s="23"/>
       <c r="J281" s="22"/>
       <c r="K281" s="22"/>
       <c r="L281" s="22"/>
@@ -8591,7 +8570,6 @@
         <v>17856</v>
       </c>
       <c r="H283" s="22"/>
-      <c r="I283" s="23"/>
       <c r="J283" s="22"/>
       <c r="K283" s="22"/>
       <c r="L283" s="22"/>

</xml_diff>